<commit_message>
New features added: 1. OpenfoamHandler with two parameters: a) -test for directing to testing directories and b) -keep_last to keep the last openfoam results for inspection; 2. Extended selection of output parameters in the output-par sheet of Masterfile
</commit_message>
<xml_diff>
--- a/test_simulation_data/Masterfile.xlsx
+++ b/test_simulation_data/Masterfile.xlsx
@@ -5,13 +5,14 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="par-cartesian" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="par-manual" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="par-random" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="par-output" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="41">
   <si>
     <t xml:space="preserve">PARAMETER</t>
   </si>
@@ -40,7 +41,7 @@
     <t xml:space="preserve">mode</t>
   </si>
   <si>
-    <t xml:space="preserve">cartesian</t>
+    <t xml:space="preserve">random</t>
   </si>
   <si>
     <t xml:space="preserve">N_random</t>
@@ -134,6 +135,18 @@
   </si>
   <si>
     <t xml:space="preserve">uniform</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OUTPUT_NAME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PATH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">magU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/postProcessing/probes/0/mag(U)</t>
   </si>
 </sst>
 </file>
@@ -210,12 +223,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -238,8 +255,8 @@
   </sheetPr>
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E26" activeCellId="0" sqref="E26"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L8" activeCellId="0" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -276,10 +293,10 @@
         <v>6</v>
       </c>
       <c r="B4" s="0" t="n">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>7</v>
       </c>
@@ -581,4 +598,65 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="25.15"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Error with output_label overfilling fixed
</commit_message>
<xml_diff>
--- a/test_simulation_data/Masterfile.xlsx
+++ b/test_simulation_data/Masterfile.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" state="visible" r:id="rId2"/>
@@ -255,8 +255,8 @@
   </sheetPr>
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L8" activeCellId="0" sqref="L8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -293,7 +293,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -607,7 +607,7 @@
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>

</xml_diff>